<commit_message>
adding other growth rate estimates
</commit_message>
<xml_diff>
--- a/d_fits.xlsx
+++ b/d_fits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jto208/Library/CloudStorage/OneDrive-UniversityofExeter/Pc paper/prochl_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{16F620F8-E438-FA4B-B55F-1FE023FC655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BC91D2A9-5EEB-784E-B835-1D966FA0B30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15860"/>
   </bookViews>
@@ -255,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,12 +465,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -632,14 +626,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -997,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="D323" sqref="D323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4289,26 +4282,26 @@
         <v>20.92</v>
       </c>
     </row>
-    <row r="144" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="6">
+    <row r="144" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
         <v>274</v>
       </c>
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C144" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D144" s="6" t="s">
+      <c r="C144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E144" s="6">
+      <c r="E144" s="1">
         <v>-9.5626094481051105</v>
       </c>
-      <c r="F144" s="6">
+      <c r="F144" s="1">
         <v>20.4373905518949</v>
       </c>
-      <c r="G144" s="6">
+      <c r="G144" s="1">
         <v>21.75</v>
       </c>
     </row>

</xml_diff>